<commit_message>
Added method to compute funded status
</commit_message>
<xml_diff>
--- a/data/plan_inputs/weights.xlsx
+++ b/data/plan_inputs/weights.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NVG9HXP\Documents\Projects\UPS_MV\data\plan_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FA12B1E-3EF7-4ACF-97C5-8656FA092A82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521E0D2B-DCE4-4733-82F9-C4539EA18AA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6915" yWindow="2715" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{1556AE39-1ADD-4B06-86A6-EDAC1302B271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{1556AE39-1ADD-4B06-86A6-EDAC1302B271}"/>
   </bookViews>
   <sheets>
     <sheet name="IBT" sheetId="1" r:id="rId1"/>
@@ -47,15 +47,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="13">
   <si>
     <t>Asset/Liability</t>
   </si>
   <si>
     <t>Weights</t>
-  </si>
-  <si>
-    <t>Factor Loadings</t>
   </si>
   <si>
     <t>Liability</t>
@@ -2774,148 +2771,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BCA4944-66DB-485D-8CD8-1B5FFDBB6057}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>-1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C3">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C4">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.43</v>
       </c>
-      <c r="C6">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0.09</v>
       </c>
-      <c r="C7">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>0.08</v>
       </c>
-      <c r="C8">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0.05</v>
       </c>
-      <c r="C9">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0.05</v>
       </c>
-      <c r="C10">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0.02</v>
       </c>
-      <c r="C11">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1.02</v>
       </c>
     </row>
   </sheetData>
@@ -2925,148 +2885,111 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D72B5F-0945-40A0-B2B2-6713E201A5C7}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>-1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C3">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C4">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.43</v>
       </c>
-      <c r="C6">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0.09</v>
       </c>
-      <c r="C7">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>0.08</v>
       </c>
-      <c r="C8">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0.05</v>
       </c>
-      <c r="C9">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0.05</v>
       </c>
-      <c r="C10">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0.02</v>
       </c>
-      <c r="C11">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1.02</v>
       </c>
     </row>
   </sheetData>
@@ -3076,148 +2999,111 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{815E1575-F746-451A-A8B2-496961B564C2}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A12"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
       </c>
       <c r="B2">
         <v>-1</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C3">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C4">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>0.43</v>
       </c>
-      <c r="C6">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>0.09</v>
       </c>
-      <c r="C7">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8">
         <v>0.08</v>
       </c>
-      <c r="C8">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>0.05</v>
       </c>
-      <c r="C9">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>0.05</v>
       </c>
-      <c r="C10">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <v>0.02</v>
       </c>
-      <c r="C11">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12">
         <v>0</v>
-      </c>
-      <c r="C12">
-        <v>1.02</v>
       </c>
     </row>
   </sheetData>

</xml_diff>